<commit_message>
Update on 20250925 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/IPV6直播源汇总/移动ITV-域名版.xlsx
+++ b/直播源汇总文档/IPV6直播源汇总/移动ITV-域名版.xlsx
@@ -19,7 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">地方!$A$1:$D$44</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">湖南!$A$1:$D$37</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">上海!$A$1:$D$103</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">体育!$A$1:$D$160</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">体育!$A$1:$D$158</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">卫视!$A$1:$D$353</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$D$265</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">娱乐!$A$1:$D$357</definedName>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5236" uniqueCount="991">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5228" uniqueCount="992">
   <si>
     <t>,</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3495,114 +3495,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>咪视通-1</t>
-  </si>
-  <si>
-    <t>咪视通-2</t>
-  </si>
-  <si>
-    <t>咪视通-3</t>
-  </si>
-  <si>
-    <t>咪视通-4</t>
-  </si>
-  <si>
-    <t>咪视通-5</t>
-  </si>
-  <si>
-    <t>咪视通-6</t>
-  </si>
-  <si>
-    <t>咪视通-7</t>
-  </si>
-  <si>
-    <t>咪视通-8</t>
-  </si>
-  <si>
-    <t>咪视通-9</t>
-  </si>
-  <si>
-    <t>咪视通-10</t>
-  </si>
-  <si>
-    <t>咪视通-11</t>
-  </si>
-  <si>
-    <t>咪视通-12</t>
-  </si>
-  <si>
-    <t>咪视通-13</t>
-  </si>
-  <si>
-    <t>咪视通-14</t>
-  </si>
-  <si>
-    <t>咪视通-15</t>
-  </si>
-  <si>
-    <t>咪视通-16</t>
-  </si>
-  <si>
-    <t>咪视通-17</t>
-  </si>
-  <si>
-    <t>咪视通-18</t>
-  </si>
-  <si>
-    <t>咪视通-19</t>
-  </si>
-  <si>
-    <t>咪视通-20</t>
-  </si>
-  <si>
-    <t>咪视通-21</t>
-  </si>
-  <si>
-    <t>咪视通-22</t>
-  </si>
-  <si>
-    <t>咪视通-23</t>
-  </si>
-  <si>
-    <t>咪视通-24</t>
-  </si>
-  <si>
-    <t>咪视通-25</t>
-  </si>
-  <si>
-    <t>咪视通-26</t>
-  </si>
-  <si>
-    <t>咪视通-27</t>
-  </si>
-  <si>
-    <t>咪视通-28</t>
-  </si>
-  <si>
-    <t>咪视通-29</t>
-  </si>
-  <si>
-    <t>咪视通-30</t>
-  </si>
-  <si>
-    <t>咪视通-31</t>
-  </si>
-  <si>
-    <t>咪视通-33</t>
-  </si>
-  <si>
-    <t>咪视通-34</t>
-  </si>
-  <si>
-    <t>咪视通-35</t>
-  </si>
-  <si>
-    <t>咪视通-3D</t>
-  </si>
-  <si>
-    <t>咪视通-4K</t>
-  </si>
-  <si>
     <t>安多卫视</t>
   </si>
   <si>
@@ -3675,9 +3567,6 @@
     <t>百视通直播-20</t>
   </si>
   <si>
-    <t>咪视通-32</t>
-  </si>
-  <si>
     <t>乐游</t>
   </si>
   <si>
@@ -3837,20 +3726,6 @@
     <t>IHOT爱院线</t>
   </si>
   <si>
-    <t>咪视通-38</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>咪视通-39</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>咪视通-36</t>
-  </si>
-  <si>
-    <t>咪视通-37</t>
-  </si>
-  <si>
     <t>,</t>
   </si>
   <si>
@@ -3870,6 +3745,133 @@
   </si>
   <si>
     <t>id=3000000001000005969</t>
+  </si>
+  <si>
+    <t>咪视界-1</t>
+  </si>
+  <si>
+    <t>咪视界-2</t>
+  </si>
+  <si>
+    <t>咪视界-3</t>
+  </si>
+  <si>
+    <t>咪视界-4</t>
+  </si>
+  <si>
+    <t>咪视界-5</t>
+  </si>
+  <si>
+    <t>咪视界-6</t>
+  </si>
+  <si>
+    <t>咪视界-7</t>
+  </si>
+  <si>
+    <t>咪视界-8</t>
+  </si>
+  <si>
+    <t>咪视界-9</t>
+  </si>
+  <si>
+    <t>咪视界-10</t>
+  </si>
+  <si>
+    <t>咪视界-11</t>
+  </si>
+  <si>
+    <t>咪视界-12</t>
+  </si>
+  <si>
+    <t>咪视界-13</t>
+  </si>
+  <si>
+    <t>咪视界-14</t>
+  </si>
+  <si>
+    <t>咪视界-15</t>
+  </si>
+  <si>
+    <t>咪视界-16</t>
+  </si>
+  <si>
+    <t>咪视界-17</t>
+  </si>
+  <si>
+    <t>咪视界-18</t>
+  </si>
+  <si>
+    <t>咪视界-19</t>
+  </si>
+  <si>
+    <t>咪视界-20</t>
+  </si>
+  <si>
+    <t>咪视界-21</t>
+  </si>
+  <si>
+    <t>咪视界-22</t>
+  </si>
+  <si>
+    <t>咪视界-23</t>
+  </si>
+  <si>
+    <t>咪视界-24</t>
+  </si>
+  <si>
+    <t>咪视界-25</t>
+  </si>
+  <si>
+    <t>咪视界-26</t>
+  </si>
+  <si>
+    <t>咪视界-27</t>
+  </si>
+  <si>
+    <t>咪视界-28</t>
+  </si>
+  <si>
+    <t>咪视界-29</t>
+  </si>
+  <si>
+    <t>咪视界-30</t>
+  </si>
+  <si>
+    <t>咪视界-31</t>
+  </si>
+  <si>
+    <t>咪视界-32</t>
+  </si>
+  <si>
+    <t>咪视界-33</t>
+  </si>
+  <si>
+    <t>咪视界-34</t>
+  </si>
+  <si>
+    <t>咪视界-35</t>
+  </si>
+  <si>
+    <t>咪视界-36</t>
+  </si>
+  <si>
+    <t>咪视界-37</t>
+  </si>
+  <si>
+    <t>咪视界-38</t>
+  </si>
+  <si>
+    <t>咪视界-39</t>
+  </si>
+  <si>
+    <t>至臻视界</t>
+  </si>
+  <si>
+    <t>咪视界-4K-1</t>
+  </si>
+  <si>
+    <t>咪视界-4K-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4251,7 +4253,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
@@ -8005,7 +8007,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>902</v>
+        <v>866</v>
       </c>
       <c r="B2" t="s">
         <v>98</v>
@@ -8019,7 +8021,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>902</v>
+        <v>866</v>
       </c>
       <c r="B3" t="s">
         <v>98</v>
@@ -8033,7 +8035,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>902</v>
+        <v>866</v>
       </c>
       <c r="B4" t="s">
         <v>98</v>
@@ -8047,7 +8049,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>902</v>
+        <v>866</v>
       </c>
       <c r="B5" t="s">
         <v>98</v>
@@ -8061,7 +8063,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>902</v>
+        <v>866</v>
       </c>
       <c r="B6" t="s">
         <v>98</v>
@@ -8075,7 +8077,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>902</v>
+        <v>866</v>
       </c>
       <c r="B7" t="s">
         <v>98</v>
@@ -8565,7 +8567,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>905</v>
+        <v>869</v>
       </c>
       <c r="B42" t="s">
         <v>98</v>
@@ -8579,7 +8581,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>905</v>
+        <v>869</v>
       </c>
       <c r="B43" t="s">
         <v>98</v>
@@ -8593,7 +8595,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>905</v>
+        <v>869</v>
       </c>
       <c r="B44" t="s">
         <v>98</v>
@@ -8607,7 +8609,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>905</v>
+        <v>869</v>
       </c>
       <c r="B45" t="s">
         <v>98</v>
@@ -8621,7 +8623,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>905</v>
+        <v>869</v>
       </c>
       <c r="B46" t="s">
         <v>98</v>
@@ -8635,7 +8637,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>905</v>
+        <v>869</v>
       </c>
       <c r="B47" t="s">
         <v>98</v>
@@ -8649,7 +8651,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>905</v>
+        <v>869</v>
       </c>
       <c r="B48" t="s">
         <v>98</v>
@@ -8663,7 +8665,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>905</v>
+        <v>869</v>
       </c>
       <c r="B49" t="s">
         <v>98</v>
@@ -8677,7 +8679,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>905</v>
+        <v>869</v>
       </c>
       <c r="B50" t="s">
         <v>98</v>
@@ -8691,7 +8693,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>905</v>
+        <v>869</v>
       </c>
       <c r="B51" t="s">
         <v>98</v>
@@ -10777,7 +10779,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A200" t="s">
-        <v>904</v>
+        <v>868</v>
       </c>
       <c r="B200" t="s">
         <v>9</v>
@@ -10791,7 +10793,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A201" t="s">
-        <v>904</v>
+        <v>868</v>
       </c>
       <c r="B201" t="s">
         <v>9</v>
@@ -10805,7 +10807,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A202" t="s">
-        <v>904</v>
+        <v>868</v>
       </c>
       <c r="B202" t="s">
         <v>9</v>
@@ -10819,7 +10821,7 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A203" t="s">
-        <v>904</v>
+        <v>868</v>
       </c>
       <c r="B203" t="s">
         <v>9</v>
@@ -10833,7 +10835,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A204" t="s">
-        <v>904</v>
+        <v>868</v>
       </c>
       <c r="B204" t="s">
         <v>9</v>
@@ -10847,7 +10849,7 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A205" t="s">
-        <v>904</v>
+        <v>868</v>
       </c>
       <c r="B205" t="s">
         <v>9</v>
@@ -11141,7 +11143,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A226" t="s">
-        <v>903</v>
+        <v>867</v>
       </c>
       <c r="B226" t="s">
         <v>7</v>
@@ -11155,7 +11157,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A227" t="s">
-        <v>903</v>
+        <v>867</v>
       </c>
       <c r="B227" t="s">
         <v>7</v>
@@ -11169,7 +11171,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A228" t="s">
-        <v>903</v>
+        <v>867</v>
       </c>
       <c r="B228" t="s">
         <v>7</v>
@@ -11183,7 +11185,7 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A229" t="s">
-        <v>903</v>
+        <v>867</v>
       </c>
       <c r="B229" t="s">
         <v>7</v>
@@ -13532,7 +13534,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>927</v>
+        <v>890</v>
       </c>
       <c r="B52" t="s">
         <v>7</v>
@@ -13546,7 +13548,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>927</v>
+        <v>890</v>
       </c>
       <c r="B53" t="s">
         <v>7</v>
@@ -13560,7 +13562,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>927</v>
+        <v>890</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
@@ -13574,7 +13576,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
-        <v>927</v>
+        <v>890</v>
       </c>
       <c r="B55" t="s">
         <v>7</v>
@@ -13588,7 +13590,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>927</v>
+        <v>890</v>
       </c>
       <c r="B56" t="s">
         <v>7</v>
@@ -13602,7 +13604,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>927</v>
+        <v>890</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
@@ -13616,7 +13618,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>927</v>
+        <v>890</v>
       </c>
       <c r="B58" t="s">
         <v>7</v>
@@ -13630,7 +13632,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
-        <v>927</v>
+        <v>890</v>
       </c>
       <c r="B59" t="s">
         <v>7</v>
@@ -15444,7 +15446,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D160"/>
+  <dimension ref="A1:D158"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -15948,7 +15950,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>866</v>
+        <v>950</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>7</v>
@@ -15962,7 +15964,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>866</v>
+        <v>950</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>7</v>
@@ -15976,7 +15978,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>867</v>
+        <v>951</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>7</v>
@@ -15990,7 +15992,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>867</v>
+        <v>951</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>7</v>
@@ -16004,7 +16006,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>868</v>
+        <v>952</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>7</v>
@@ -16018,7 +16020,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>868</v>
+        <v>952</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>7</v>
@@ -16032,7 +16034,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>869</v>
+        <v>953</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>7</v>
@@ -16046,7 +16048,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>869</v>
+        <v>953</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>7</v>
@@ -16060,7 +16062,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>870</v>
+        <v>954</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>7</v>
@@ -16074,7 +16076,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>870</v>
+        <v>954</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>7</v>
@@ -16088,7 +16090,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>871</v>
+        <v>955</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>7</v>
@@ -16102,7 +16104,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>871</v>
+        <v>955</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>7</v>
@@ -16116,7 +16118,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>872</v>
+        <v>956</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>7</v>
@@ -16130,7 +16132,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>872</v>
+        <v>956</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>7</v>
@@ -16144,7 +16146,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>873</v>
+        <v>957</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>7</v>
@@ -16158,7 +16160,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>873</v>
+        <v>957</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>7</v>
@@ -16172,7 +16174,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>874</v>
+        <v>958</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>7</v>
@@ -16186,7 +16188,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>874</v>
+        <v>958</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>7</v>
@@ -16200,7 +16202,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>875</v>
+        <v>959</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>7</v>
@@ -16214,7 +16216,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>875</v>
+        <v>959</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>7</v>
@@ -16228,7 +16230,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>876</v>
+        <v>960</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>7</v>
@@ -16242,7 +16244,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
-        <v>876</v>
+        <v>960</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>7</v>
@@ -16256,7 +16258,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>877</v>
+        <v>961</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>7</v>
@@ -16270,7 +16272,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>877</v>
+        <v>961</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>7</v>
@@ -16284,7 +16286,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>878</v>
+        <v>962</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>7</v>
@@ -16298,7 +16300,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
-        <v>878</v>
+        <v>962</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>7</v>
@@ -16312,7 +16314,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>879</v>
+        <v>963</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>7</v>
@@ -16326,7 +16328,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
-        <v>879</v>
+        <v>963</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>7</v>
@@ -16340,7 +16342,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
-        <v>880</v>
+        <v>964</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>7</v>
@@ -16354,7 +16356,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
-        <v>880</v>
+        <v>964</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>7</v>
@@ -16368,7 +16370,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
-        <v>881</v>
+        <v>965</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>7</v>
@@ -16382,7 +16384,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
-        <v>881</v>
+        <v>965</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>7</v>
@@ -16396,7 +16398,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
-        <v>882</v>
+        <v>966</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>7</v>
@@ -16410,7 +16412,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>882</v>
+        <v>966</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>7</v>
@@ -16424,7 +16426,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>883</v>
+        <v>967</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>7</v>
@@ -16438,7 +16440,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
-        <v>883</v>
+        <v>967</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>7</v>
@@ -16452,7 +16454,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
-        <v>884</v>
+        <v>968</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>7</v>
@@ -16466,7 +16468,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
-        <v>884</v>
+        <v>968</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>7</v>
@@ -16480,7 +16482,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
-        <v>885</v>
+        <v>969</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>7</v>
@@ -16494,7 +16496,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
-        <v>885</v>
+        <v>969</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>7</v>
@@ -16508,7 +16510,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
-        <v>886</v>
+        <v>970</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>7</v>
@@ -16522,7 +16524,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
-        <v>886</v>
+        <v>970</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>7</v>
@@ -16536,7 +16538,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
-        <v>887</v>
+        <v>971</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>7</v>
@@ -16550,7 +16552,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
-        <v>887</v>
+        <v>971</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>7</v>
@@ -16564,7 +16566,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
-        <v>888</v>
+        <v>972</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>7</v>
@@ -16578,7 +16580,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
-        <v>888</v>
+        <v>972</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>7</v>
@@ -16592,7 +16594,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
-        <v>889</v>
+        <v>973</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>7</v>
@@ -16606,7 +16608,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
-        <v>889</v>
+        <v>973</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>7</v>
@@ -16620,7 +16622,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
-        <v>890</v>
+        <v>974</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>7</v>
@@ -16634,7 +16636,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
-        <v>890</v>
+        <v>974</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>7</v>
@@ -16648,7 +16650,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
-        <v>891</v>
+        <v>975</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>7</v>
@@ -16662,7 +16664,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
-        <v>891</v>
+        <v>975</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>7</v>
@@ -16676,7 +16678,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
-        <v>892</v>
+        <v>976</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>7</v>
@@ -16690,7 +16692,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
-        <v>892</v>
+        <v>976</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>7</v>
@@ -16704,7 +16706,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
-        <v>893</v>
+        <v>977</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>7</v>
@@ -16718,7 +16720,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
-        <v>893</v>
+        <v>977</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>7</v>
@@ -16732,7 +16734,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
-        <v>894</v>
+        <v>978</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>7</v>
@@ -16746,7 +16748,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
-        <v>894</v>
+        <v>978</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>7</v>
@@ -16760,7 +16762,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
-        <v>895</v>
+        <v>979</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>7</v>
@@ -16774,7 +16776,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A95" s="1" t="s">
-        <v>895</v>
+        <v>979</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>7</v>
@@ -16788,7 +16790,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A96" s="1" t="s">
-        <v>896</v>
+        <v>980</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>7</v>
@@ -16802,7 +16804,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A97" s="1" t="s">
-        <v>896</v>
+        <v>980</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>7</v>
@@ -16816,7 +16818,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
-        <v>926</v>
+        <v>981</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>7</v>
@@ -16830,7 +16832,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
-        <v>926</v>
+        <v>981</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>7</v>
@@ -16844,7 +16846,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
-        <v>897</v>
+        <v>982</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>7</v>
@@ -16858,7 +16860,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
-        <v>897</v>
+        <v>982</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>7</v>
@@ -16872,119 +16874,119 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
-        <v>898</v>
+        <v>983</v>
       </c>
       <c r="B102" t="s">
-        <v>984</v>
+        <v>943</v>
       </c>
       <c r="C102" t="s">
-        <v>985</v>
+        <v>944</v>
       </c>
       <c r="D102" t="s">
-        <v>986</v>
+        <v>945</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
-        <v>898</v>
+        <v>983</v>
       </c>
       <c r="B103" t="s">
-        <v>984</v>
+        <v>943</v>
       </c>
       <c r="C103" t="s">
-        <v>987</v>
+        <v>946</v>
       </c>
       <c r="D103" t="s">
-        <v>986</v>
+        <v>945</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
-        <v>899</v>
+        <v>984</v>
       </c>
       <c r="B104" t="s">
-        <v>984</v>
+        <v>943</v>
       </c>
       <c r="C104" t="s">
-        <v>985</v>
+        <v>944</v>
       </c>
       <c r="D104" t="s">
-        <v>988</v>
+        <v>947</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
-        <v>899</v>
+        <v>984</v>
       </c>
       <c r="B105" t="s">
-        <v>984</v>
+        <v>943</v>
       </c>
       <c r="C105" t="s">
-        <v>987</v>
+        <v>946</v>
       </c>
       <c r="D105" t="s">
-        <v>988</v>
+        <v>947</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
-        <v>982</v>
+        <v>985</v>
       </c>
       <c r="B106" t="s">
-        <v>984</v>
+        <v>943</v>
       </c>
       <c r="C106" t="s">
-        <v>985</v>
+        <v>944</v>
       </c>
       <c r="D106" t="s">
-        <v>989</v>
+        <v>948</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
-        <v>982</v>
+        <v>985</v>
       </c>
       <c r="B107" t="s">
-        <v>984</v>
+        <v>943</v>
       </c>
       <c r="C107" t="s">
-        <v>987</v>
+        <v>946</v>
       </c>
       <c r="D107" t="s">
-        <v>989</v>
+        <v>948</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
-        <v>983</v>
+        <v>986</v>
       </c>
       <c r="B108" t="s">
-        <v>984</v>
+        <v>943</v>
       </c>
       <c r="C108" t="s">
-        <v>985</v>
+        <v>944</v>
       </c>
       <c r="D108" t="s">
-        <v>990</v>
+        <v>949</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
-        <v>983</v>
+        <v>986</v>
       </c>
       <c r="B109" t="s">
-        <v>984</v>
+        <v>943</v>
       </c>
       <c r="C109" t="s">
-        <v>987</v>
+        <v>946</v>
       </c>
       <c r="D109" t="s">
-        <v>990</v>
+        <v>949</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A110" s="1" t="s">
-        <v>980</v>
+        <v>987</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>7</v>
@@ -16998,7 +17000,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A111" s="1" t="s">
-        <v>981</v>
+        <v>988</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>7</v>
@@ -17012,7 +17014,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A112" s="1" t="s">
-        <v>981</v>
+        <v>988</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>7</v>
@@ -17026,7 +17028,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A113" s="1" t="s">
-        <v>900</v>
+        <v>989</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>7</v>
@@ -17040,7 +17042,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
-        <v>900</v>
+        <v>989</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>7</v>
@@ -17054,7 +17056,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A115" s="1" t="s">
-        <v>900</v>
+        <v>990</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>7</v>
@@ -17063,12 +17065,12 @@
         <v>13</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A116" s="1" t="s">
-        <v>900</v>
+        <v>990</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>7</v>
@@ -17077,12 +17079,12 @@
         <v>14</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A117" s="1" t="s">
-        <v>901</v>
+        <v>991</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>7</v>
@@ -17091,12 +17093,12 @@
         <v>13</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A118" s="1" t="s">
-        <v>901</v>
+        <v>991</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>7</v>
@@ -17105,40 +17107,40 @@
         <v>14</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A119" s="1" t="s">
-        <v>901</v>
+        <v>870</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A120" s="1" t="s">
-        <v>901</v>
+        <v>870</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A121" s="1" t="s">
-        <v>906</v>
+        <v>871</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>7</v>
@@ -17147,12 +17149,12 @@
         <v>11</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A122" s="1" t="s">
-        <v>906</v>
+        <v>871</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>7</v>
@@ -17161,12 +17163,12 @@
         <v>12</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
-        <v>907</v>
+        <v>872</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>7</v>
@@ -17175,12 +17177,12 @@
         <v>11</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A124" s="1" t="s">
-        <v>907</v>
+        <v>872</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>7</v>
@@ -17189,12 +17191,12 @@
         <v>12</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A125" s="1" t="s">
-        <v>908</v>
+        <v>873</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>7</v>
@@ -17203,12 +17205,12 @@
         <v>11</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A126" s="1" t="s">
-        <v>908</v>
+        <v>873</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>7</v>
@@ -17217,12 +17219,12 @@
         <v>12</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A127" s="1" t="s">
-        <v>909</v>
+        <v>874</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>7</v>
@@ -17231,12 +17233,12 @@
         <v>11</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A128" s="1" t="s">
-        <v>909</v>
+        <v>874</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>7</v>
@@ -17245,12 +17247,12 @@
         <v>12</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A129" s="1" t="s">
-        <v>910</v>
+        <v>875</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>7</v>
@@ -17259,12 +17261,12 @@
         <v>11</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
-        <v>910</v>
+        <v>875</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>7</v>
@@ -17273,12 +17275,12 @@
         <v>12</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A131" s="1" t="s">
-        <v>911</v>
+        <v>876</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>7</v>
@@ -17287,12 +17289,12 @@
         <v>11</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A132" s="1" t="s">
-        <v>911</v>
+        <v>876</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>7</v>
@@ -17301,12 +17303,12 @@
         <v>12</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A133" s="1" t="s">
-        <v>912</v>
+        <v>877</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>7</v>
@@ -17315,12 +17317,12 @@
         <v>11</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A134" s="1" t="s">
-        <v>912</v>
+        <v>877</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>7</v>
@@ -17329,12 +17331,12 @@
         <v>12</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A135" s="1" t="s">
-        <v>913</v>
+        <v>878</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>7</v>
@@ -17343,12 +17345,12 @@
         <v>11</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
-        <v>913</v>
+        <v>878</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>7</v>
@@ -17357,12 +17359,12 @@
         <v>12</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A137" s="1" t="s">
-        <v>914</v>
+        <v>879</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>7</v>
@@ -17371,12 +17373,12 @@
         <v>11</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A138" s="1" t="s">
-        <v>914</v>
+        <v>879</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>7</v>
@@ -17385,40 +17387,40 @@
         <v>12</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
-        <v>915</v>
+        <v>880</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>11</v>
+        <v>84</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A140" s="1" t="s">
-        <v>915</v>
+        <v>880</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A141" s="1" t="s">
-        <v>916</v>
+        <v>881</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>7</v>
@@ -17427,12 +17429,12 @@
         <v>84</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A142" s="1" t="s">
-        <v>916</v>
+        <v>881</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>7</v>
@@ -17441,12 +17443,12 @@
         <v>86</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A143" s="1" t="s">
-        <v>917</v>
+        <v>882</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>7</v>
@@ -17455,12 +17457,12 @@
         <v>84</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A144" s="1" t="s">
-        <v>917</v>
+        <v>882</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>7</v>
@@ -17469,12 +17471,12 @@
         <v>86</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A145" s="1" t="s">
-        <v>918</v>
+        <v>883</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>7</v>
@@ -17483,12 +17485,12 @@
         <v>84</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A146" s="1" t="s">
-        <v>918</v>
+        <v>883</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>7</v>
@@ -17497,12 +17499,12 @@
         <v>86</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A147" s="1" t="s">
-        <v>919</v>
+        <v>884</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>7</v>
@@ -17511,12 +17513,12 @@
         <v>84</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A148" s="1" t="s">
-        <v>919</v>
+        <v>884</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>7</v>
@@ -17525,12 +17527,12 @@
         <v>86</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A149" s="1" t="s">
-        <v>920</v>
+        <v>885</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>7</v>
@@ -17539,12 +17541,12 @@
         <v>84</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A150" s="1" t="s">
-        <v>920</v>
+        <v>885</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>7</v>
@@ -17553,12 +17555,12 @@
         <v>86</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A151" s="1" t="s">
-        <v>921</v>
+        <v>886</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>7</v>
@@ -17567,12 +17569,12 @@
         <v>84</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A152" s="1" t="s">
-        <v>921</v>
+        <v>886</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>7</v>
@@ -17581,12 +17583,12 @@
         <v>86</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A153" s="1" t="s">
-        <v>922</v>
+        <v>887</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>7</v>
@@ -17595,12 +17597,12 @@
         <v>84</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A154" s="1" t="s">
-        <v>922</v>
+        <v>887</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>7</v>
@@ -17609,12 +17611,12 @@
         <v>86</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A155" s="1" t="s">
-        <v>923</v>
+        <v>888</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>7</v>
@@ -17623,12 +17625,12 @@
         <v>84</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A156" s="1" t="s">
-        <v>923</v>
+        <v>888</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>7</v>
@@ -17637,12 +17639,12 @@
         <v>86</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A157" s="1" t="s">
-        <v>924</v>
+        <v>889</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>7</v>
@@ -17651,12 +17653,12 @@
         <v>84</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A158" s="1" t="s">
-        <v>924</v>
+        <v>889</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>7</v>
@@ -17665,39 +17667,11 @@
         <v>86</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A159" s="1" t="s">
-        <v>925</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D159" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A160" s="1" t="s">
-        <v>925</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D160"/>
+  <autoFilter ref="A1:D158"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -18350,7 +18324,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>960</v>
+        <v>923</v>
       </c>
       <c r="B46" t="s">
         <v>7</v>
@@ -18364,7 +18338,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>960</v>
+        <v>923</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
@@ -18378,7 +18352,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>960</v>
+        <v>923</v>
       </c>
       <c r="B48" t="s">
         <v>7</v>
@@ -18392,7 +18366,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>960</v>
+        <v>923</v>
       </c>
       <c r="B49" t="s">
         <v>7</v>
@@ -18406,7 +18380,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>961</v>
+        <v>924</v>
       </c>
       <c r="B50" t="s">
         <v>7</v>
@@ -18420,7 +18394,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>961</v>
+        <v>924</v>
       </c>
       <c r="B51" t="s">
         <v>7</v>
@@ -18434,7 +18408,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>961</v>
+        <v>924</v>
       </c>
       <c r="B52" t="s">
         <v>7</v>
@@ -18448,7 +18422,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>961</v>
+        <v>924</v>
       </c>
       <c r="B53" t="s">
         <v>7</v>
@@ -18462,7 +18436,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>962</v>
+        <v>925</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
@@ -18476,7 +18450,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
-        <v>962</v>
+        <v>925</v>
       </c>
       <c r="B55" t="s">
         <v>7</v>
@@ -18490,7 +18464,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>962</v>
+        <v>925</v>
       </c>
       <c r="B56" t="s">
         <v>7</v>
@@ -18504,7 +18478,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>962</v>
+        <v>925</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
@@ -18518,7 +18492,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>963</v>
+        <v>926</v>
       </c>
       <c r="B58" t="s">
         <v>7</v>
@@ -18532,7 +18506,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
-        <v>963</v>
+        <v>926</v>
       </c>
       <c r="B59" t="s">
         <v>7</v>
@@ -18546,7 +18520,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
-        <v>964</v>
+        <v>927</v>
       </c>
       <c r="B60" t="s">
         <v>7</v>
@@ -18560,7 +18534,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>964</v>
+        <v>927</v>
       </c>
       <c r="B61" t="s">
         <v>7</v>
@@ -18574,7 +18548,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
-        <v>964</v>
+        <v>927</v>
       </c>
       <c r="B62" t="s">
         <v>7</v>
@@ -18588,7 +18562,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
-        <v>964</v>
+        <v>927</v>
       </c>
       <c r="B63" t="s">
         <v>7</v>
@@ -18602,7 +18576,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
-        <v>965</v>
+        <v>928</v>
       </c>
       <c r="B64" t="s">
         <v>7</v>
@@ -18616,7 +18590,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
-        <v>965</v>
+        <v>928</v>
       </c>
       <c r="B65" t="s">
         <v>7</v>
@@ -18630,7 +18604,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
-        <v>965</v>
+        <v>928</v>
       </c>
       <c r="B66" t="s">
         <v>7</v>
@@ -18644,7 +18618,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
-        <v>965</v>
+        <v>928</v>
       </c>
       <c r="B67" t="s">
         <v>7</v>
@@ -18658,7 +18632,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
-        <v>966</v>
+        <v>929</v>
       </c>
       <c r="B68" t="s">
         <v>7</v>
@@ -18672,7 +18646,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
-        <v>966</v>
+        <v>929</v>
       </c>
       <c r="B69" t="s">
         <v>7</v>
@@ -18686,7 +18660,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
-        <v>966</v>
+        <v>929</v>
       </c>
       <c r="B70" t="s">
         <v>7</v>
@@ -18700,7 +18674,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
-        <v>966</v>
+        <v>929</v>
       </c>
       <c r="B71" t="s">
         <v>7</v>
@@ -18714,7 +18688,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
-        <v>967</v>
+        <v>930</v>
       </c>
       <c r="B72" t="s">
         <v>7</v>
@@ -18728,7 +18702,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
-        <v>967</v>
+        <v>930</v>
       </c>
       <c r="B73" t="s">
         <v>7</v>
@@ -18742,7 +18716,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
-        <v>967</v>
+        <v>930</v>
       </c>
       <c r="B74" t="s">
         <v>7</v>
@@ -18756,7 +18730,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
-        <v>967</v>
+        <v>930</v>
       </c>
       <c r="B75" t="s">
         <v>7</v>
@@ -18770,7 +18744,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
-        <v>968</v>
+        <v>931</v>
       </c>
       <c r="B76" t="s">
         <v>7</v>
@@ -18784,7 +18758,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
-        <v>968</v>
+        <v>931</v>
       </c>
       <c r="B77" t="s">
         <v>7</v>
@@ -18798,7 +18772,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
-        <v>968</v>
+        <v>931</v>
       </c>
       <c r="B78" t="s">
         <v>7</v>
@@ -18812,7 +18786,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
-        <v>968</v>
+        <v>931</v>
       </c>
       <c r="B79" t="s">
         <v>7</v>
@@ -18826,7 +18800,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
-        <v>969</v>
+        <v>932</v>
       </c>
       <c r="B80" t="s">
         <v>7</v>
@@ -18840,7 +18814,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
-        <v>969</v>
+        <v>932</v>
       </c>
       <c r="B81" t="s">
         <v>7</v>
@@ -18854,7 +18828,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
-        <v>969</v>
+        <v>932</v>
       </c>
       <c r="B82" t="s">
         <v>7</v>
@@ -18868,7 +18842,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
-        <v>969</v>
+        <v>932</v>
       </c>
       <c r="B83" t="s">
         <v>7</v>
@@ -18882,7 +18856,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
-        <v>970</v>
+        <v>933</v>
       </c>
       <c r="B84" t="s">
         <v>7</v>
@@ -18896,7 +18870,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
-        <v>970</v>
+        <v>933</v>
       </c>
       <c r="B85" t="s">
         <v>7</v>
@@ -18910,7 +18884,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
-        <v>970</v>
+        <v>933</v>
       </c>
       <c r="B86" t="s">
         <v>7</v>
@@ -18924,7 +18898,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
-        <v>970</v>
+        <v>933</v>
       </c>
       <c r="B87" t="s">
         <v>7</v>
@@ -18938,7 +18912,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
-        <v>971</v>
+        <v>934</v>
       </c>
       <c r="B88" t="s">
         <v>7</v>
@@ -18952,7 +18926,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
-        <v>971</v>
+        <v>934</v>
       </c>
       <c r="B89" t="s">
         <v>7</v>
@@ -18966,7 +18940,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
-        <v>971</v>
+        <v>934</v>
       </c>
       <c r="B90" t="s">
         <v>7</v>
@@ -18980,7 +18954,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
-        <v>971</v>
+        <v>934</v>
       </c>
       <c r="B91" t="s">
         <v>7</v>
@@ -18994,7 +18968,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
-        <v>972</v>
+        <v>935</v>
       </c>
       <c r="B92" t="s">
         <v>7</v>
@@ -19008,7 +18982,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
-        <v>972</v>
+        <v>935</v>
       </c>
       <c r="B93" t="s">
         <v>7</v>
@@ -19022,7 +18996,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
-        <v>972</v>
+        <v>935</v>
       </c>
       <c r="B94" t="s">
         <v>7</v>
@@ -19036,7 +19010,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
-        <v>972</v>
+        <v>935</v>
       </c>
       <c r="B95" t="s">
         <v>7</v>
@@ -19050,7 +19024,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
-        <v>973</v>
+        <v>936</v>
       </c>
       <c r="B96" t="s">
         <v>7</v>
@@ -19064,7 +19038,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
-        <v>973</v>
+        <v>936</v>
       </c>
       <c r="B97" t="s">
         <v>7</v>
@@ -19078,7 +19052,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
-        <v>973</v>
+        <v>936</v>
       </c>
       <c r="B98" t="s">
         <v>7</v>
@@ -19092,7 +19066,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
-        <v>973</v>
+        <v>936</v>
       </c>
       <c r="B99" t="s">
         <v>7</v>
@@ -19106,7 +19080,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A100" t="s">
-        <v>974</v>
+        <v>937</v>
       </c>
       <c r="B100" t="s">
         <v>7</v>
@@ -19120,7 +19094,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
-        <v>974</v>
+        <v>937</v>
       </c>
       <c r="B101" t="s">
         <v>7</v>
@@ -19134,7 +19108,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
-        <v>974</v>
+        <v>937</v>
       </c>
       <c r="B102" t="s">
         <v>7</v>
@@ -19148,7 +19122,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
-        <v>974</v>
+        <v>937</v>
       </c>
       <c r="B103" t="s">
         <v>7</v>
@@ -19162,7 +19136,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
-        <v>975</v>
+        <v>938</v>
       </c>
       <c r="B104" t="s">
         <v>7</v>
@@ -19176,7 +19150,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
-        <v>975</v>
+        <v>938</v>
       </c>
       <c r="B105" t="s">
         <v>7</v>
@@ -19190,7 +19164,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
-        <v>975</v>
+        <v>938</v>
       </c>
       <c r="B106" t="s">
         <v>7</v>
@@ -19204,7 +19178,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
-        <v>975</v>
+        <v>938</v>
       </c>
       <c r="B107" t="s">
         <v>7</v>
@@ -19218,7 +19192,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
-        <v>976</v>
+        <v>939</v>
       </c>
       <c r="B108" t="s">
         <v>7</v>
@@ -19232,7 +19206,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
-        <v>976</v>
+        <v>939</v>
       </c>
       <c r="B109" t="s">
         <v>7</v>
@@ -19246,7 +19220,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
-        <v>976</v>
+        <v>939</v>
       </c>
       <c r="B110" t="s">
         <v>7</v>
@@ -19260,7 +19234,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
-        <v>976</v>
+        <v>939</v>
       </c>
       <c r="B111" t="s">
         <v>7</v>
@@ -19274,7 +19248,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
-        <v>977</v>
+        <v>940</v>
       </c>
       <c r="B112" t="s">
         <v>7</v>
@@ -19288,7 +19262,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
-        <v>977</v>
+        <v>940</v>
       </c>
       <c r="B113" t="s">
         <v>7</v>
@@ -19302,7 +19276,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
-        <v>977</v>
+        <v>940</v>
       </c>
       <c r="B114" t="s">
         <v>7</v>
@@ -19316,7 +19290,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
-        <v>977</v>
+        <v>940</v>
       </c>
       <c r="B115" t="s">
         <v>7</v>
@@ -19330,7 +19304,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A116" t="s">
-        <v>978</v>
+        <v>941</v>
       </c>
       <c r="B116" t="s">
         <v>7</v>
@@ -19344,7 +19318,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
-        <v>978</v>
+        <v>941</v>
       </c>
       <c r="B117" t="s">
         <v>7</v>
@@ -19358,7 +19332,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A118" t="s">
-        <v>978</v>
+        <v>941</v>
       </c>
       <c r="B118" t="s">
         <v>7</v>
@@ -19372,7 +19346,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A119" t="s">
-        <v>978</v>
+        <v>941</v>
       </c>
       <c r="B119" t="s">
         <v>7</v>
@@ -19386,7 +19360,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A120" t="s">
-        <v>979</v>
+        <v>942</v>
       </c>
       <c r="B120" t="s">
         <v>7</v>
@@ -19400,7 +19374,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A121" t="s">
-        <v>979</v>
+        <v>942</v>
       </c>
       <c r="B121" t="s">
         <v>7</v>
@@ -19414,7 +19388,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A122" t="s">
-        <v>979</v>
+        <v>942</v>
       </c>
       <c r="B122" t="s">
         <v>7</v>
@@ -19428,7 +19402,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A123" t="s">
-        <v>979</v>
+        <v>942</v>
       </c>
       <c r="B123" t="s">
         <v>7</v>
@@ -19442,7 +19416,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A124" t="s">
-        <v>928</v>
+        <v>891</v>
       </c>
       <c r="B124" t="s">
         <v>7</v>
@@ -19456,7 +19430,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A125" t="s">
-        <v>928</v>
+        <v>891</v>
       </c>
       <c r="B125" t="s">
         <v>7</v>
@@ -19470,7 +19444,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A126" t="s">
-        <v>928</v>
+        <v>891</v>
       </c>
       <c r="B126" t="s">
         <v>7</v>
@@ -19484,7 +19458,7 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A127" t="s">
-        <v>928</v>
+        <v>891</v>
       </c>
       <c r="B127" t="s">
         <v>7</v>
@@ -19498,7 +19472,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A128" t="s">
-        <v>929</v>
+        <v>892</v>
       </c>
       <c r="B128" t="s">
         <v>7</v>
@@ -19512,7 +19486,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A129" t="s">
-        <v>929</v>
+        <v>892</v>
       </c>
       <c r="B129" t="s">
         <v>7</v>
@@ -19526,7 +19500,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A130" t="s">
-        <v>929</v>
+        <v>892</v>
       </c>
       <c r="B130" t="s">
         <v>7</v>
@@ -19540,7 +19514,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A131" t="s">
-        <v>929</v>
+        <v>892</v>
       </c>
       <c r="B131" t="s">
         <v>7</v>
@@ -19554,7 +19528,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A132" t="s">
-        <v>929</v>
+        <v>892</v>
       </c>
       <c r="B132" t="s">
         <v>7</v>
@@ -19568,7 +19542,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A133" t="s">
-        <v>929</v>
+        <v>892</v>
       </c>
       <c r="B133" t="s">
         <v>7</v>
@@ -19582,7 +19556,7 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A134" t="s">
-        <v>929</v>
+        <v>892</v>
       </c>
       <c r="B134" t="s">
         <v>7</v>
@@ -19596,7 +19570,7 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A135" t="s">
-        <v>929</v>
+        <v>892</v>
       </c>
       <c r="B135" t="s">
         <v>7</v>
@@ -19610,7 +19584,7 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A136" t="s">
-        <v>930</v>
+        <v>893</v>
       </c>
       <c r="B136" t="s">
         <v>7</v>
@@ -19624,7 +19598,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A137" t="s">
-        <v>930</v>
+        <v>893</v>
       </c>
       <c r="B137" t="s">
         <v>7</v>
@@ -19638,7 +19612,7 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A138" t="s">
-        <v>930</v>
+        <v>893</v>
       </c>
       <c r="B138" t="s">
         <v>7</v>
@@ -19652,7 +19626,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A139" t="s">
-        <v>930</v>
+        <v>893</v>
       </c>
       <c r="B139" t="s">
         <v>7</v>
@@ -19666,7 +19640,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A140" t="s">
-        <v>930</v>
+        <v>893</v>
       </c>
       <c r="B140" t="s">
         <v>7</v>
@@ -19680,7 +19654,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A141" t="s">
-        <v>930</v>
+        <v>893</v>
       </c>
       <c r="B141" t="s">
         <v>7</v>
@@ -19694,7 +19668,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A142" t="s">
-        <v>930</v>
+        <v>893</v>
       </c>
       <c r="B142" t="s">
         <v>7</v>
@@ -19708,7 +19682,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A143" t="s">
-        <v>930</v>
+        <v>893</v>
       </c>
       <c r="B143" t="s">
         <v>7</v>
@@ -19722,7 +19696,7 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A144" t="s">
-        <v>931</v>
+        <v>894</v>
       </c>
       <c r="B144" t="s">
         <v>7</v>
@@ -19736,7 +19710,7 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A145" t="s">
-        <v>931</v>
+        <v>894</v>
       </c>
       <c r="B145" t="s">
         <v>7</v>
@@ -19750,7 +19724,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A146" t="s">
-        <v>931</v>
+        <v>894</v>
       </c>
       <c r="B146" t="s">
         <v>7</v>
@@ -19764,7 +19738,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A147" t="s">
-        <v>931</v>
+        <v>894</v>
       </c>
       <c r="B147" t="s">
         <v>7</v>
@@ -19778,7 +19752,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A148" t="s">
-        <v>931</v>
+        <v>894</v>
       </c>
       <c r="B148" t="s">
         <v>7</v>
@@ -19792,7 +19766,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A149" t="s">
-        <v>931</v>
+        <v>894</v>
       </c>
       <c r="B149" t="s">
         <v>7</v>
@@ -19806,7 +19780,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A150" t="s">
-        <v>931</v>
+        <v>894</v>
       </c>
       <c r="B150" t="s">
         <v>7</v>
@@ -19820,7 +19794,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A151" t="s">
-        <v>931</v>
+        <v>894</v>
       </c>
       <c r="B151" t="s">
         <v>9</v>
@@ -19834,7 +19808,7 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A152" t="s">
-        <v>932</v>
+        <v>895</v>
       </c>
       <c r="B152" t="s">
         <v>7</v>
@@ -19848,7 +19822,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A153" t="s">
-        <v>932</v>
+        <v>895</v>
       </c>
       <c r="B153" t="s">
         <v>7</v>
@@ -19862,7 +19836,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A154" t="s">
-        <v>932</v>
+        <v>895</v>
       </c>
       <c r="B154" t="s">
         <v>7</v>
@@ -19876,7 +19850,7 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A155" t="s">
-        <v>932</v>
+        <v>895</v>
       </c>
       <c r="B155" t="s">
         <v>7</v>
@@ -19890,7 +19864,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A156" t="s">
-        <v>932</v>
+        <v>895</v>
       </c>
       <c r="B156" t="s">
         <v>7</v>
@@ -19904,7 +19878,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A157" t="s">
-        <v>932</v>
+        <v>895</v>
       </c>
       <c r="B157" t="s">
         <v>7</v>
@@ -19918,7 +19892,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A158" t="s">
-        <v>932</v>
+        <v>895</v>
       </c>
       <c r="B158" t="s">
         <v>7</v>
@@ -19932,7 +19906,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A159" t="s">
-        <v>932</v>
+        <v>895</v>
       </c>
       <c r="B159" t="s">
         <v>7</v>
@@ -19946,7 +19920,7 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A160" t="s">
-        <v>933</v>
+        <v>896</v>
       </c>
       <c r="B160" t="s">
         <v>7</v>
@@ -19960,7 +19934,7 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A161" t="s">
-        <v>933</v>
+        <v>896</v>
       </c>
       <c r="B161" t="s">
         <v>7</v>
@@ -19974,7 +19948,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A162" t="s">
-        <v>933</v>
+        <v>896</v>
       </c>
       <c r="B162" t="s">
         <v>7</v>
@@ -19988,7 +19962,7 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A163" t="s">
-        <v>933</v>
+        <v>896</v>
       </c>
       <c r="B163" t="s">
         <v>7</v>
@@ -20002,7 +19976,7 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A164" t="s">
-        <v>934</v>
+        <v>897</v>
       </c>
       <c r="B164" t="s">
         <v>7</v>
@@ -20016,7 +19990,7 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A165" t="s">
-        <v>934</v>
+        <v>897</v>
       </c>
       <c r="B165" t="s">
         <v>7</v>
@@ -20030,7 +20004,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A166" t="s">
-        <v>934</v>
+        <v>897</v>
       </c>
       <c r="B166" t="s">
         <v>7</v>
@@ -20044,7 +20018,7 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A167" t="s">
-        <v>934</v>
+        <v>897</v>
       </c>
       <c r="B167" t="s">
         <v>7</v>
@@ -20058,7 +20032,7 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A168" t="s">
-        <v>935</v>
+        <v>898</v>
       </c>
       <c r="B168" t="s">
         <v>7</v>
@@ -20072,7 +20046,7 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A169" t="s">
-        <v>935</v>
+        <v>898</v>
       </c>
       <c r="B169" t="s">
         <v>7</v>
@@ -20086,7 +20060,7 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A170" t="s">
-        <v>935</v>
+        <v>898</v>
       </c>
       <c r="B170" t="s">
         <v>7</v>
@@ -20100,7 +20074,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A171" t="s">
-        <v>935</v>
+        <v>898</v>
       </c>
       <c r="B171" t="s">
         <v>7</v>
@@ -20114,7 +20088,7 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A172" t="s">
-        <v>935</v>
+        <v>898</v>
       </c>
       <c r="B172" t="s">
         <v>7</v>
@@ -20128,7 +20102,7 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A173" t="s">
-        <v>935</v>
+        <v>898</v>
       </c>
       <c r="B173" t="s">
         <v>7</v>
@@ -20142,7 +20116,7 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A174" t="s">
-        <v>935</v>
+        <v>898</v>
       </c>
       <c r="B174" t="s">
         <v>7</v>
@@ -20156,7 +20130,7 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A175" t="s">
-        <v>935</v>
+        <v>898</v>
       </c>
       <c r="B175" t="s">
         <v>7</v>
@@ -20170,7 +20144,7 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A176" t="s">
-        <v>935</v>
+        <v>898</v>
       </c>
       <c r="B176" t="s">
         <v>7</v>
@@ -20184,7 +20158,7 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A177" t="s">
-        <v>935</v>
+        <v>898</v>
       </c>
       <c r="B177" t="s">
         <v>7</v>
@@ -20198,7 +20172,7 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A178" t="s">
-        <v>935</v>
+        <v>898</v>
       </c>
       <c r="B178" t="s">
         <v>7</v>
@@ -20212,7 +20186,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A179" t="s">
-        <v>935</v>
+        <v>898</v>
       </c>
       <c r="B179" t="s">
         <v>7</v>
@@ -20226,7 +20200,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A180" t="s">
-        <v>936</v>
+        <v>899</v>
       </c>
       <c r="B180" t="s">
         <v>7</v>
@@ -20240,7 +20214,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A181" t="s">
-        <v>936</v>
+        <v>899</v>
       </c>
       <c r="B181" t="s">
         <v>7</v>
@@ -20254,7 +20228,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A182" t="s">
-        <v>936</v>
+        <v>899</v>
       </c>
       <c r="B182" t="s">
         <v>7</v>
@@ -20268,7 +20242,7 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A183" t="s">
-        <v>936</v>
+        <v>899</v>
       </c>
       <c r="B183" t="s">
         <v>7</v>
@@ -20282,7 +20256,7 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A184" t="s">
-        <v>937</v>
+        <v>900</v>
       </c>
       <c r="B184" t="s">
         <v>7</v>
@@ -20296,7 +20270,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A185" t="s">
-        <v>937</v>
+        <v>900</v>
       </c>
       <c r="B185" t="s">
         <v>7</v>
@@ -20310,7 +20284,7 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A186" t="s">
-        <v>937</v>
+        <v>900</v>
       </c>
       <c r="B186" t="s">
         <v>7</v>
@@ -20324,7 +20298,7 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A187" t="s">
-        <v>937</v>
+        <v>900</v>
       </c>
       <c r="B187" t="s">
         <v>7</v>
@@ -20338,7 +20312,7 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A188" t="s">
-        <v>937</v>
+        <v>900</v>
       </c>
       <c r="B188" t="s">
         <v>7</v>
@@ -20352,7 +20326,7 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A189" t="s">
-        <v>937</v>
+        <v>900</v>
       </c>
       <c r="B189" t="s">
         <v>7</v>
@@ -20366,7 +20340,7 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A190" t="s">
-        <v>938</v>
+        <v>901</v>
       </c>
       <c r="B190" t="s">
         <v>7</v>
@@ -20380,7 +20354,7 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A191" t="s">
-        <v>938</v>
+        <v>901</v>
       </c>
       <c r="B191" t="s">
         <v>7</v>
@@ -20394,7 +20368,7 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A192" t="s">
-        <v>938</v>
+        <v>901</v>
       </c>
       <c r="B192" t="s">
         <v>7</v>
@@ -20408,7 +20382,7 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A193" t="s">
-        <v>938</v>
+        <v>901</v>
       </c>
       <c r="B193" t="s">
         <v>7</v>
@@ -20422,7 +20396,7 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A194" t="s">
-        <v>939</v>
+        <v>902</v>
       </c>
       <c r="B194" t="s">
         <v>7</v>
@@ -20436,7 +20410,7 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A195" t="s">
-        <v>939</v>
+        <v>902</v>
       </c>
       <c r="B195" t="s">
         <v>7</v>
@@ -20450,7 +20424,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A196" t="s">
-        <v>939</v>
+        <v>902</v>
       </c>
       <c r="B196" t="s">
         <v>7</v>
@@ -20464,7 +20438,7 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A197" t="s">
-        <v>939</v>
+        <v>902</v>
       </c>
       <c r="B197" t="s">
         <v>7</v>
@@ -20478,7 +20452,7 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A198" t="s">
-        <v>939</v>
+        <v>902</v>
       </c>
       <c r="B198" t="s">
         <v>7</v>
@@ -20492,7 +20466,7 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A199" t="s">
-        <v>939</v>
+        <v>902</v>
       </c>
       <c r="B199" t="s">
         <v>7</v>
@@ -20506,7 +20480,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A200" t="s">
-        <v>940</v>
+        <v>903</v>
       </c>
       <c r="B200" t="s">
         <v>7</v>
@@ -20520,7 +20494,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A201" t="s">
-        <v>940</v>
+        <v>903</v>
       </c>
       <c r="B201" t="s">
         <v>7</v>
@@ -20534,7 +20508,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A202" t="s">
-        <v>940</v>
+        <v>903</v>
       </c>
       <c r="B202" t="s">
         <v>7</v>
@@ -20548,7 +20522,7 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A203" t="s">
-        <v>940</v>
+        <v>903</v>
       </c>
       <c r="B203" t="s">
         <v>7</v>
@@ -20562,7 +20536,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A204" t="s">
-        <v>940</v>
+        <v>903</v>
       </c>
       <c r="B204" t="s">
         <v>7</v>
@@ -20576,7 +20550,7 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A205" t="s">
-        <v>940</v>
+        <v>903</v>
       </c>
       <c r="B205" t="s">
         <v>7</v>
@@ -20590,7 +20564,7 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A206" t="s">
-        <v>941</v>
+        <v>904</v>
       </c>
       <c r="B206" t="s">
         <v>7</v>
@@ -20604,7 +20578,7 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A207" t="s">
-        <v>941</v>
+        <v>904</v>
       </c>
       <c r="B207" t="s">
         <v>7</v>
@@ -20618,7 +20592,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A208" t="s">
-        <v>941</v>
+        <v>904</v>
       </c>
       <c r="B208" t="s">
         <v>7</v>
@@ -20632,7 +20606,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A209" t="s">
-        <v>941</v>
+        <v>904</v>
       </c>
       <c r="B209" t="s">
         <v>7</v>
@@ -20646,7 +20620,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A210" t="s">
-        <v>942</v>
+        <v>905</v>
       </c>
       <c r="B210" t="s">
         <v>7</v>
@@ -20660,7 +20634,7 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A211" t="s">
-        <v>942</v>
+        <v>905</v>
       </c>
       <c r="B211" t="s">
         <v>7</v>
@@ -20674,7 +20648,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A212" t="s">
-        <v>942</v>
+        <v>905</v>
       </c>
       <c r="B212" t="s">
         <v>7</v>
@@ -20688,7 +20662,7 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A213" t="s">
-        <v>942</v>
+        <v>905</v>
       </c>
       <c r="B213" t="s">
         <v>7</v>
@@ -20702,7 +20676,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A214" t="s">
-        <v>942</v>
+        <v>905</v>
       </c>
       <c r="B214" t="s">
         <v>7</v>
@@ -20716,7 +20690,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A215" t="s">
-        <v>942</v>
+        <v>905</v>
       </c>
       <c r="B215" t="s">
         <v>7</v>
@@ -20730,7 +20704,7 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A216" t="s">
-        <v>943</v>
+        <v>906</v>
       </c>
       <c r="B216" t="s">
         <v>7</v>
@@ -20744,7 +20718,7 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A217" t="s">
-        <v>943</v>
+        <v>906</v>
       </c>
       <c r="B217" t="s">
         <v>7</v>
@@ -20758,7 +20732,7 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A218" t="s">
-        <v>943</v>
+        <v>906</v>
       </c>
       <c r="B218" t="s">
         <v>7</v>
@@ -20772,7 +20746,7 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A219" t="s">
-        <v>943</v>
+        <v>906</v>
       </c>
       <c r="B219" t="s">
         <v>7</v>
@@ -20786,7 +20760,7 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A220" t="s">
-        <v>943</v>
+        <v>906</v>
       </c>
       <c r="B220" t="s">
         <v>7</v>
@@ -20800,7 +20774,7 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A221" t="s">
-        <v>943</v>
+        <v>906</v>
       </c>
       <c r="B221" t="s">
         <v>7</v>
@@ -20814,7 +20788,7 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A222" t="s">
-        <v>944</v>
+        <v>907</v>
       </c>
       <c r="B222" t="s">
         <v>7</v>
@@ -20828,7 +20802,7 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A223" t="s">
-        <v>944</v>
+        <v>907</v>
       </c>
       <c r="B223" t="s">
         <v>7</v>
@@ -20842,7 +20816,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A224" t="s">
-        <v>944</v>
+        <v>907</v>
       </c>
       <c r="B224" t="s">
         <v>7</v>
@@ -20856,7 +20830,7 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A225" t="s">
-        <v>944</v>
+        <v>907</v>
       </c>
       <c r="B225" t="s">
         <v>7</v>
@@ -20870,7 +20844,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A226" t="s">
-        <v>944</v>
+        <v>907</v>
       </c>
       <c r="B226" t="s">
         <v>7</v>
@@ -20884,7 +20858,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A227" t="s">
-        <v>944</v>
+        <v>907</v>
       </c>
       <c r="B227" t="s">
         <v>7</v>
@@ -20898,7 +20872,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A228" t="s">
-        <v>945</v>
+        <v>908</v>
       </c>
       <c r="B228" t="s">
         <v>7</v>
@@ -20912,7 +20886,7 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A229" t="s">
-        <v>945</v>
+        <v>908</v>
       </c>
       <c r="B229" t="s">
         <v>7</v>
@@ -20926,7 +20900,7 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A230" t="s">
-        <v>945</v>
+        <v>908</v>
       </c>
       <c r="B230" t="s">
         <v>7</v>
@@ -20940,7 +20914,7 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A231" t="s">
-        <v>945</v>
+        <v>908</v>
       </c>
       <c r="B231" t="s">
         <v>7</v>
@@ -20954,7 +20928,7 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A232" t="s">
-        <v>945</v>
+        <v>908</v>
       </c>
       <c r="B232" t="s">
         <v>7</v>
@@ -20968,7 +20942,7 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A233" t="s">
-        <v>945</v>
+        <v>908</v>
       </c>
       <c r="B233" t="s">
         <v>7</v>
@@ -20982,7 +20956,7 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A234" t="s">
-        <v>946</v>
+        <v>909</v>
       </c>
       <c r="B234" t="s">
         <v>7</v>
@@ -20996,7 +20970,7 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A235" t="s">
-        <v>946</v>
+        <v>909</v>
       </c>
       <c r="B235" t="s">
         <v>7</v>
@@ -21010,7 +20984,7 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A236" t="s">
-        <v>946</v>
+        <v>909</v>
       </c>
       <c r="B236" t="s">
         <v>7</v>
@@ -21024,7 +20998,7 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A237" t="s">
-        <v>946</v>
+        <v>909</v>
       </c>
       <c r="B237" t="s">
         <v>7</v>
@@ -21038,7 +21012,7 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A238" t="s">
-        <v>947</v>
+        <v>910</v>
       </c>
       <c r="B238" t="s">
         <v>7</v>
@@ -21052,7 +21026,7 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A239" t="s">
-        <v>947</v>
+        <v>910</v>
       </c>
       <c r="B239" t="s">
         <v>7</v>
@@ -21066,7 +21040,7 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A240" t="s">
-        <v>947</v>
+        <v>910</v>
       </c>
       <c r="B240" t="s">
         <v>7</v>
@@ -21080,7 +21054,7 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A241" t="s">
-        <v>947</v>
+        <v>910</v>
       </c>
       <c r="B241" t="s">
         <v>7</v>
@@ -21094,7 +21068,7 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A242" t="s">
-        <v>948</v>
+        <v>911</v>
       </c>
       <c r="B242" t="s">
         <v>7</v>
@@ -21108,7 +21082,7 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A243" t="s">
-        <v>948</v>
+        <v>911</v>
       </c>
       <c r="B243" t="s">
         <v>7</v>
@@ -21122,7 +21096,7 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A244" t="s">
-        <v>948</v>
+        <v>911</v>
       </c>
       <c r="B244" t="s">
         <v>7</v>
@@ -21136,7 +21110,7 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A245" t="s">
-        <v>948</v>
+        <v>911</v>
       </c>
       <c r="B245" t="s">
         <v>7</v>
@@ -21150,7 +21124,7 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A246" t="s">
-        <v>948</v>
+        <v>911</v>
       </c>
       <c r="B246" t="s">
         <v>7</v>
@@ -21164,7 +21138,7 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A247" t="s">
-        <v>948</v>
+        <v>911</v>
       </c>
       <c r="B247" t="s">
         <v>7</v>
@@ -21178,7 +21152,7 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A248" t="s">
-        <v>949</v>
+        <v>912</v>
       </c>
       <c r="B248" t="s">
         <v>7</v>
@@ -21192,7 +21166,7 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A249" t="s">
-        <v>949</v>
+        <v>912</v>
       </c>
       <c r="B249" t="s">
         <v>7</v>
@@ -21206,7 +21180,7 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A250" t="s">
-        <v>949</v>
+        <v>912</v>
       </c>
       <c r="B250" t="s">
         <v>7</v>
@@ -21220,7 +21194,7 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A251" t="s">
-        <v>949</v>
+        <v>912</v>
       </c>
       <c r="B251" t="s">
         <v>7</v>
@@ -21234,7 +21208,7 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A252" t="s">
-        <v>949</v>
+        <v>912</v>
       </c>
       <c r="B252" t="s">
         <v>7</v>
@@ -21248,7 +21222,7 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A253" t="s">
-        <v>949</v>
+        <v>912</v>
       </c>
       <c r="B253" t="s">
         <v>7</v>
@@ -21262,7 +21236,7 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A254" t="s">
-        <v>950</v>
+        <v>913</v>
       </c>
       <c r="B254" t="s">
         <v>7</v>
@@ -21276,7 +21250,7 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A255" t="s">
-        <v>950</v>
+        <v>913</v>
       </c>
       <c r="B255" t="s">
         <v>7</v>
@@ -21290,7 +21264,7 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A256" t="s">
-        <v>950</v>
+        <v>913</v>
       </c>
       <c r="B256" t="s">
         <v>7</v>
@@ -21304,7 +21278,7 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A257" t="s">
-        <v>950</v>
+        <v>913</v>
       </c>
       <c r="B257" t="s">
         <v>7</v>
@@ -21318,7 +21292,7 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A258" t="s">
-        <v>951</v>
+        <v>914</v>
       </c>
       <c r="B258" t="s">
         <v>7</v>
@@ -21332,7 +21306,7 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A259" t="s">
-        <v>951</v>
+        <v>914</v>
       </c>
       <c r="B259" t="s">
         <v>7</v>
@@ -21346,7 +21320,7 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A260" t="s">
-        <v>951</v>
+        <v>914</v>
       </c>
       <c r="B260" t="s">
         <v>7</v>
@@ -21360,7 +21334,7 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A261" t="s">
-        <v>951</v>
+        <v>914</v>
       </c>
       <c r="B261" t="s">
         <v>7</v>
@@ -21374,7 +21348,7 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A262" t="s">
-        <v>952</v>
+        <v>915</v>
       </c>
       <c r="B262" t="s">
         <v>7</v>
@@ -21388,7 +21362,7 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A263" t="s">
-        <v>952</v>
+        <v>915</v>
       </c>
       <c r="B263" t="s">
         <v>7</v>
@@ -21402,7 +21376,7 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A264" t="s">
-        <v>952</v>
+        <v>915</v>
       </c>
       <c r="B264" t="s">
         <v>7</v>
@@ -21416,7 +21390,7 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A265" t="s">
-        <v>952</v>
+        <v>915</v>
       </c>
       <c r="B265" t="s">
         <v>7</v>
@@ -21430,7 +21404,7 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A266" t="s">
-        <v>952</v>
+        <v>915</v>
       </c>
       <c r="B266" t="s">
         <v>7</v>
@@ -21444,7 +21418,7 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A267" t="s">
-        <v>952</v>
+        <v>915</v>
       </c>
       <c r="B267" t="s">
         <v>7</v>
@@ -21458,7 +21432,7 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A268" t="s">
-        <v>953</v>
+        <v>916</v>
       </c>
       <c r="B268" t="s">
         <v>7</v>
@@ -21472,7 +21446,7 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A269" t="s">
-        <v>953</v>
+        <v>916</v>
       </c>
       <c r="B269" t="s">
         <v>7</v>
@@ -21486,7 +21460,7 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A270" t="s">
-        <v>954</v>
+        <v>917</v>
       </c>
       <c r="B270" t="s">
         <v>7</v>
@@ -21500,7 +21474,7 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A271" t="s">
-        <v>954</v>
+        <v>917</v>
       </c>
       <c r="B271" t="s">
         <v>7</v>
@@ -21514,7 +21488,7 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A272" t="s">
-        <v>954</v>
+        <v>917</v>
       </c>
       <c r="B272" t="s">
         <v>7</v>
@@ -21528,7 +21502,7 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A273" t="s">
-        <v>954</v>
+        <v>917</v>
       </c>
       <c r="B273" t="s">
         <v>7</v>
@@ -21542,7 +21516,7 @@
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A274" t="s">
-        <v>955</v>
+        <v>918</v>
       </c>
       <c r="B274" t="s">
         <v>7</v>
@@ -21556,7 +21530,7 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A275" t="s">
-        <v>955</v>
+        <v>918</v>
       </c>
       <c r="B275" t="s">
         <v>7</v>
@@ -21570,7 +21544,7 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A276" t="s">
-        <v>956</v>
+        <v>919</v>
       </c>
       <c r="B276" t="s">
         <v>7</v>
@@ -21584,7 +21558,7 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A277" t="s">
-        <v>956</v>
+        <v>919</v>
       </c>
       <c r="B277" t="s">
         <v>7</v>
@@ -21598,7 +21572,7 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A278" t="s">
-        <v>956</v>
+        <v>919</v>
       </c>
       <c r="B278" t="s">
         <v>7</v>
@@ -21612,7 +21586,7 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A279" t="s">
-        <v>956</v>
+        <v>919</v>
       </c>
       <c r="B279" t="s">
         <v>7</v>
@@ -21626,7 +21600,7 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A280" t="s">
-        <v>957</v>
+        <v>920</v>
       </c>
       <c r="B280" t="s">
         <v>7</v>
@@ -21640,7 +21614,7 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A281" t="s">
-        <v>957</v>
+        <v>920</v>
       </c>
       <c r="B281" t="s">
         <v>7</v>
@@ -21654,7 +21628,7 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A282" t="s">
-        <v>957</v>
+        <v>920</v>
       </c>
       <c r="B282" t="s">
         <v>7</v>
@@ -21668,7 +21642,7 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A283" t="s">
-        <v>957</v>
+        <v>920</v>
       </c>
       <c r="B283" t="s">
         <v>7</v>
@@ -21682,7 +21656,7 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A284" t="s">
-        <v>958</v>
+        <v>921</v>
       </c>
       <c r="B284" t="s">
         <v>7</v>
@@ -21696,7 +21670,7 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A285" t="s">
-        <v>958</v>
+        <v>921</v>
       </c>
       <c r="B285" t="s">
         <v>7</v>
@@ -21710,7 +21684,7 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A286" t="s">
-        <v>958</v>
+        <v>921</v>
       </c>
       <c r="B286" t="s">
         <v>7</v>
@@ -21724,7 +21698,7 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A287" t="s">
-        <v>958</v>
+        <v>921</v>
       </c>
       <c r="B287" t="s">
         <v>7</v>
@@ -21738,7 +21712,7 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A288" t="s">
-        <v>958</v>
+        <v>921</v>
       </c>
       <c r="B288" t="s">
         <v>7</v>
@@ -21752,7 +21726,7 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A289" t="s">
-        <v>958</v>
+        <v>921</v>
       </c>
       <c r="B289" t="s">
         <v>7</v>
@@ -21766,7 +21740,7 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A290" t="s">
-        <v>959</v>
+        <v>922</v>
       </c>
       <c r="B290" t="s">
         <v>7</v>
@@ -21780,7 +21754,7 @@
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A291" t="s">
-        <v>959</v>
+        <v>922</v>
       </c>
       <c r="B291" t="s">
         <v>7</v>
@@ -21794,7 +21768,7 @@
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A292" t="s">
-        <v>959</v>
+        <v>922</v>
       </c>
       <c r="B292" t="s">
         <v>7</v>
@@ -21808,7 +21782,7 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A293" t="s">
-        <v>959</v>
+        <v>922</v>
       </c>
       <c r="B293" t="s">
         <v>7</v>

</xml_diff>